<commit_message>
documentation, changed fazit and prepared new pictures
</commit_message>
<xml_diff>
--- a/doc/thesis/pictures/konzept/solution2/algorithm.xlsx
+++ b/doc/thesis/pictures/konzept/solution2/algorithm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="6924"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Solution2_five_sto_curve_disk -" sheetId="1" r:id="rId1"/>
@@ -1250,11 +1250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363370296"/>
-        <c:axId val="363371080"/>
+        <c:axId val="218193928"/>
+        <c:axId val="218190792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363370296"/>
+        <c:axId val="218193928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,10 +1298,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1311,12 +1308,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363371080"/>
+        <c:crossAx val="218190792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363371080"/>
+        <c:axId val="218190792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,10 +1357,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1373,7 +1367,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363370296"/>
+        <c:crossAx val="218193928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1424,10 +1418,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1903,11 +1894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="270826432"/>
-        <c:axId val="270828784"/>
+        <c:axId val="218194320"/>
+        <c:axId val="218191576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="270826432"/>
+        <c:axId val="218194320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1951,10 +1942,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1964,12 +1952,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270828784"/>
+        <c:crossAx val="218191576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="270828784"/>
+        <c:axId val="218191576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,10 +2001,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2026,7 +2011,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270826432"/>
+        <c:crossAx val="218194320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2056,10 +2041,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3551,13 +3533,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -3577,7 +3559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3600,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3623,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3646,7 +3628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3669,7 +3651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3692,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3715,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3738,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3761,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3784,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3807,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3830,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3853,7 +3835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3876,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3899,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3922,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3945,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3968,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3991,12 +3973,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -4007,7 +3989,7 @@
         <v>-10037</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -4021,7 +4003,7 @@
         <v>-2817</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
@@ -4035,7 +4017,7 @@
         <v>11565</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -4046,7 +4028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -4066,7 +4048,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
changing pictures and cleaning up documentation
</commit_message>
<xml_diff>
--- a/doc/thesis/pictures/konzept/solution2/algorithm.xlsx
+++ b/doc/thesis/pictures/konzept/solution2/algorithm.xlsx
@@ -1250,11 +1250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218193928"/>
-        <c:axId val="218190792"/>
+        <c:axId val="264975648"/>
+        <c:axId val="264978000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218193928"/>
+        <c:axId val="264975648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,12 +1308,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218190792"/>
+        <c:crossAx val="264978000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218190792"/>
+        <c:axId val="264978000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +1367,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218193928"/>
+        <c:crossAx val="264975648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1894,11 +1894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218194320"/>
-        <c:axId val="218191576"/>
+        <c:axId val="264978784"/>
+        <c:axId val="264982704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218194320"/>
+        <c:axId val="264978784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1940,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1952,12 +1952,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218191576"/>
+        <c:crossAx val="264982704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218191576"/>
+        <c:axId val="264982704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +1999,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2011,7 +2011,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218194320"/>
+        <c:crossAx val="264978784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2039,7 +2039,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2084,7 +2084,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3238,13 +3238,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>464820</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>99059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133695</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3533,8 +3533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>